<commit_message>
Ajout écriture ficher excel
</commit_message>
<xml_diff>
--- a/DataAnalyse.xlsx
+++ b/DataAnalyse.xlsx
@@ -1,27 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\S4\os05\B\Calendar\Calendar\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D248BD-F4D3-4BE8-A94F-FDDD8A8D1537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+  <si>
+    <t>Matière</t>
+  </si>
+  <si>
+    <t>Salle</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Date de début</t>
+  </si>
+  <si>
+    <t>Date de fin</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>M4203C-EVAL-2-EG-SB-BD</t>
+  </si>
+  <si>
+    <t>A251 (85pl./160)</t>
+  </si>
+  <si>
+    <t>\n\nG22-S4\nGRAZIANO EMMANUELLE\nBOUCHON STÉPHANIE\nDIARD BEN</t>
+  </si>
+  <si>
+    <t>OS09A-EVAL-2</t>
+  </si>
+  <si>
+    <t>D360 (16 pl./32)</t>
+  </si>
+  <si>
+    <t>\n\nG22-S4\nDELL'AIERA MICHAEL\n(Exporté le:22/03/2022 18:44)</t>
+  </si>
+  <si>
+    <t>OS03-EVAL-FJ</t>
+  </si>
+  <si>
+    <t>\n\nG22-S4\nJAZIRI FAOUZI\n(Exporté le:22/03/2022 18:44)\n</t>
+  </si>
+  <si>
+    <t>Point stage</t>
+  </si>
+  <si>
+    <t>\n\nINFO2-S4\nGRUSON NATHALIE\n(Exporté le:22/03/2022 18:44)\</t>
+  </si>
+  <si>
+    <t>TOEIC Examen DUETI</t>
+  </si>
+  <si>
+    <t>E104 (66 pl./66)\,E102 (66 pl./66)\,E103 (50 pl./52)</t>
+  </si>
+  <si>
+    <t>\n\nINFO2-S4\nBACHELET CAROLE\n(Exporté le:22/03/2022 18:44)\</t>
+  </si>
+  <si>
+    <t>OS05B-EVAL-G22</t>
+  </si>
+  <si>
+    <t>D250 (15 pl./27)\,D251 (11 pl./22)</t>
+  </si>
+  <si>
+    <t>\n\nG22-S4\nDAMAS LUC\n(Exporté le:22/03/2022 18:44)\n</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="hh:mm:ss"/>
+  </numFmts>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -50,22 +119,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -353,13 +416,154 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44645.5</v>
+      </c>
+      <c r="E2" s="1">
+        <v>44645.58333333334</v>
+      </c>
+      <c r="F2" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44642.375</v>
+      </c>
+      <c r="E3" s="1">
+        <v>44642.45833333334</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44642.29166666666</v>
+      </c>
+      <c r="E4" s="1">
+        <v>44642.375</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.08333333333333333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44644.47916666666</v>
+      </c>
+      <c r="E5" s="1">
+        <v>44644.52083333334</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.04166666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1">
+        <v>44644.52083333334</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44644.64583333334</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44643.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>44643.66666666666</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>